<commit_message>
added excel sheet for conc tables
</commit_message>
<xml_diff>
--- a/metadata/ConcordanceTables_ANOVA.xlsx
+++ b/metadata/ConcordanceTables_ANOVA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/TimMcInerney/GitCode/MitoImputePrep/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B1534D1-7825-4B49-9A1D-3002BEAAD6C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E80AD19-E8E2-6E4D-BDB5-06BEDB9174F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="5" xr2:uid="{912AF37D-FA91-664E-A565-57F8EF0CC832}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="4" xr2:uid="{912AF37D-FA91-664E-A565-57F8EF0CC832}"/>
   </bookViews>
   <sheets>
     <sheet name="MCMC_diff_means" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="12">
   <si>
     <t>contrast</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>&lt;.0001</t>
+  </si>
+  <si>
+    <t>kHAP</t>
   </si>
 </sst>
 </file>
@@ -845,14 +848,215 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{223AC02A-7414-294E-8350-E8D031ABF7C3}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1">
+        <v>100</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.45014729999999997</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1.3199819999999999E-2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>900</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.42424129999999999</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.47605330000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1">
+        <v>250</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.4318418</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1.3199819999999999E-2</v>
+      </c>
+      <c r="D3" s="1">
+        <v>900</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.40593580000000001</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.45774779999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1">
+        <v>500</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.42694599999999999</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1.3199819999999999E-2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>900</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.40104000000000001</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.45285199999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.41775610000000002</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1.3199819999999999E-2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>900</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.39185009999999998</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.4436621</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1">
+        <v>2500</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.39016309999999998</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1.3199819999999999E-2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>900</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.3642571</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.41606910000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1">
+        <v>5000</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.2984598</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1.3199819999999999E-2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>900</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.27255380000000001</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.32436579999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1">
+        <v>10000</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.21020649999999999</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1.3199819999999999E-2</v>
+      </c>
+      <c r="D8" s="1">
+        <v>900</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.18430050000000001</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.2361125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1">
+        <v>20000</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.18133969999999999</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1.3199819999999999E-2</v>
+      </c>
+      <c r="D9" s="1">
+        <v>900</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.15543370000000001</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.2072457</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1">
+        <v>30000</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.1767917</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1.3199819999999999E-2</v>
+      </c>
+      <c r="D10" s="1">
+        <v>900</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.15088570000000001</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.20269770000000001</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -861,7 +1065,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{908BB4AE-9330-064D-A775-D615E72A203C}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G37" sqref="A1:G37"/>
     </sheetView>
   </sheetViews>

</xml_diff>